<commit_message>
Ažuriran fajl sa testovima-ZADAZAK3
</commit_message>
<xml_diff>
--- a/TESTOVI.xlsx
+++ b/TESTOVI.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19440" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Test case" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Broj testa</t>
   </si>
@@ -61,28 +61,13 @@
     </r>
   </si>
   <si>
-    <t>1. instalirana aplikacija
-2. otvoren nalog na sistemu</t>
-  </si>
-  <si>
-    <t>1. pokretanje aplikacije
-2. unos korisničkog imena i lozinke u odgovarajuća polja na formi za prijavu
-3. klik na tipku "Prijava"</t>
-  </si>
-  <si>
     <t>Prošao</t>
   </si>
   <si>
     <t>/</t>
   </si>
   <si>
-    <t>Igor</t>
-  </si>
-  <si>
     <t>Windows 7</t>
-  </si>
-  <si>
-    <t>Test case primjer</t>
   </si>
   <si>
     <t>1.инсталирана аплик
@@ -483,9 +468,6 @@
 4. Provjera da li su ispisane sve rezervacije iz foldera</t>
   </si>
   <si>
-    <t>12.02.2022.</t>
-  </si>
-  <si>
     <t>Test je prošao.
  Sve rezervacije iz foldera
  su prikazane korisniku na
@@ -605,19 +587,323 @@
 5. Napravljene su ručno rezervacije, u folderu rezervacija, koje u sebi sadrže ID leta.</t>
   </si>
   <si>
-    <t>???</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Pregled rasporeda letova(Kontrolor)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test kojim se urvđuje da li je omogućen pregled rasporede letova</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Pokretanje aplikacije
+2. Prijavljivanje na sistem kao kontrolor
+3. Unos komande --view
+</t>
+  </si>
+  <si>
+    <t>Raspored letova je pravilno prikazan na konzoli</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Otkazivanje leta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Test kojim se utvrđuje da li je omogućeno pravilno otkazivanje leta</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Prijavljivanje na sistem kao kontrolor
+3. Unos komande --decline
+4. Unos ID-a leta koji želimo otkazati
+5. Pregled liste letova komandom --view
+6. Pokušati otkazati let koji ne postoji
+7. Pokušati otkazati let koji je već poletio</t>
+  </si>
+  <si>
+    <t>Prilikom otkazivanja
+ leta ispisana greška 
+da se ne može otkazati let koji je već poletio, iako nije.</t>
+  </si>
+  <si>
+    <t>14.01.2022.</t>
+  </si>
+  <si>
+    <t>12.01.2022.</t>
+  </si>
+  <si>
+    <t>Neophodno ispraviti provjeru da li se otkazuje let koji ne postoji.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Promjena statusa leta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test kojim se utvrđuje da li kontrolor može pravilno promjeniti status leta</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Instalirana aplikacija
+2. Postoji nalog kontrolora u sistemu
+3. Kontrolor je prijavljen na sistem
+4. Postoji kreiran let</t>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Prijavljivanje na sistem kao kontrolor
+3. Unos komande --change
+4. Unos ID-a leta čiji status mjenjamo
+5.  Unos opcije Sletio/Leti/Poletio
+6. Provjera ponašanja u različitim opcijama:
+7. Ako se izabere opcija Poletio da se let upisuje u datoteku aktivnih letova
+8. Ako se izabere opcija Leti da se stanje leta pravilno ažurira u datoteci aktivnih letova kao i u datoteci leta
+9. Ako se izabere opcija Sletio da se let upisuje u datoteku završenih letova i da se briše iz datoteke aktivnih letova</t>
+  </si>
+  <si>
+    <t>Program pravilno vrši promjenu statusa leta te mjenja stanje datoteka.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Pregled izvještaja (Šef)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test kojim se utvrđuje da li šef ima opciju pregleda izvještaja na dnevnom/sedmičnom/mjesečnom nivou</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Instalirana aplikacija
+2. Postoji nalog šefa u sistemu
+3. Šef je prijavljen na sistem
+4. Postoje kreirani letovi</t>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Prijavljivanje na sistem kao šef
+3. Unos komande --viewreports
+4. Izbor opcije --daily/--weekly/--monthly za izbor nivoa
+5. Unos datuma
+6. Provjera za svaku od opcija
+7. Pokušati unijeti nepravilan datum</t>
+  </si>
+  <si>
+    <t>Pravilno izvršen prikaz na dnevnom/sedmičnom/mjesečnom nivou. Program pravilno provjerava datum i prikazuje grešku ukoliko je unijet nepostojeći datum.</t>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Prijavljivanje na sistem kao šef
+3. Unos komande --viewreservations</t>
+  </si>
+  <si>
+    <t>Tetst prošao. Uspješno prikazane sve rezervacije u sistemu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. pokretanje aplikacije
+2. unos korisničkog imena i lozinke
+3. Pokušati unijeti pogrešno ime/lozinku.
+</t>
+  </si>
+  <si>
+    <t>14.01.2022</t>
+  </si>
+  <si>
+    <t>1. instalirana aplikacija
+2. administrator je dodao nalog u sistem</t>
+  </si>
+  <si>
+    <t>Korisnici se pravilno mogu 
+prijaviti</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Odjavljivanje sa naloga
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test kojim se provjerava da li se korisnik može odjaviti sa naloga.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Instalirana aplikacija
+2. Postoji nalog u sistemu
+3. Korisnik je prijavljen</t>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Unos podataka za prijavljivanje
+3. Unos komande -logout</t>
+  </si>
+  <si>
+    <t>Korisnik se može odjaviti sa sistema.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Zatvaranje programa
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provjera da li se program može zatvoriti preko komande</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Instalirana aplikacija
+</t>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Unos komande --exit</t>
+  </si>
+  <si>
+    <t>Korisnk može prestati sa radom pomoću komande --exit</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Pregled dokumentacije
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test kojim se utvrđuje da li korisnik može pregledati dokumentaciju za svoj nalog</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Pokretanje aplikacije
+2. Unos podataka za prijavljivanje
+3. Unos komande -d ili --doc
+4. Provjera za različite tipove naloga</t>
+  </si>
+  <si>
+    <t>Pravilno prikazana dokumentacija za sve korisnike.</t>
+  </si>
+  <si>
+    <t>18:15
+14.01.2022.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -696,9 +982,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,44 +993,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1050,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1106,384 +1401,619 @@
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="6">
-        <v>43451</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
+      <c r="J2" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="78" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>14</v>
+      <c r="F3" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="174.6" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="202.15" customHeight="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>34</v>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="190.15" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="188.25" customHeight="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="G8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="107.25" customHeight="1">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="120.75" customHeight="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>52</v>
+      <c r="J10" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="B11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>57</v>
+      <c r="J11" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="16" t="s">
+      <c r="B12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="J12" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>54</v>
+      <c r="B13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>64</v>
+      <c r="J13" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>67</v>
       </c>
+      <c r="G15" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="17" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="18" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="19" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="20" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="21" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="22" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="23" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="24" s="3" customFormat="1" ht="60" customHeight="1"/>
-    <row r="25" ht="60" customHeight="1"/>
-    <row r="26" ht="60" customHeight="1"/>
-    <row r="27" ht="60" customHeight="1"/>
-    <row r="28" ht="60" customHeight="1"/>
-    <row r="29" ht="60" customHeight="1"/>
-    <row r="30" ht="60" customHeight="1"/>
-    <row r="31" ht="60" customHeight="1"/>
-    <row r="32" ht="60" customHeight="1"/>
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
+    <row r="24" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1"/>
+    <row r="25" spans="1:10" ht="60" customHeight="1"/>
+    <row r="26" spans="1:10" ht="60" customHeight="1"/>
+    <row r="27" spans="1:10" ht="60" customHeight="1"/>
+    <row r="28" spans="1:10" ht="60" customHeight="1"/>
+    <row r="29" spans="1:10" ht="60" customHeight="1"/>
+    <row r="30" spans="1:10" ht="60" customHeight="1"/>
+    <row r="31" spans="1:10" ht="60" customHeight="1"/>
+    <row r="32" spans="1:10" ht="60" customHeight="1"/>
     <row r="33" ht="60" customHeight="1"/>
     <row r="34" ht="60" customHeight="1"/>
     <row r="35" ht="60" customHeight="1"/>

</xml_diff>